<commit_message>
se suben los archivos datasources para los endosos
</commit_message>
<xml_diff>
--- a/Sura/Endoso_Modificacion_De_Coberturas.xlsx
+++ b/Sura/Endoso_Modificacion_De_Coberturas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A9E260-51DB-44F6-9639-A38933A07713}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE900409-77D5-44A0-AC71-FBA5721FED0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
     <t>04104012812</t>
   </si>
   <si>
-    <t>04104013194</t>
+    <t>04104016434</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>